<commit_message>
fix requests_method about put and delete
</commit_message>
<xml_diff>
--- a/TestCase/test.xlsx
+++ b/TestCase/test.xlsx
@@ -60,7 +60,21 @@
     <t>POST</t>
   </si>
   <si>
-    <t>{"doorBanSn":"1111","ip":"1.1.1.1","doorBanName":"门禁1","manufacturer":"厂商1","model":"型号1","longitude":120.333,"latitude":20.333,"regionCode":"330104","communityCode":"330104","direction":"0","installationAddress":"杭州下去","remark":"没有备注","state":0}</t>
+    <t>{
+"doorBanSn":"1111",
+"ip":"1.1.1.1",
+"doorBanName":"门禁1",
+"manufacturer":"厂商1",
+"model":"型号1",
+"longitude":120.333,
+"latitude":20.333,
+"regionCode":"330104",
+"communityCode":"330104",
+"direction":"0",
+"installationAddress":"杭州下去",
+"remark":"没有备注",
+"state":0
+}</t>
   </si>
   <si>
     <t>根据小区编码与状态值查询门禁机列表</t>
@@ -85,7 +99,7 @@
     <t>仅必填参数</t>
   </si>
   <si>
-    <t>http://181.181.0.33:22020/api/acs/v1/door_ban/</t>
+    <t>http://181.181.0.33:22020/api/acs/v1/door_ban/?id=66</t>
   </si>
   <si>
     <t>DELETE</t>
@@ -101,20 +115,20 @@
   </si>
   <si>
     <t>{
- "id":${id},
- "doorBanSn":"222",
- "ip":"2.2.2.2",
- "doorBanName":"门禁2",
- "manufacturer":"厂商2",
- "model":"型号2",
- "longitude":20.333,
- "latitude":120.333,
- "regionCode":"110227",
- "communityCode":"110101570B48",
- "direction":"1",
- "installationAddress":"杭州上去",
- "remark":"有备注",
- "state":1
+"id":"68",
+"doorBanSn":"2222",
+"ip":"2.2.2.2",
+"doorBanName":"门禁1",
+"manufacturer":"厂商1",
+"model":"型号1",
+"longitude":120.333,
+"latitude":20.333,
+"regionCode":"330104",
+"communityCode":"330104",
+"direction":"0",
+"installationAddress":"杭州下去",
+"remark":"没有备注",
+"state":0
 }</t>
   </si>
 </sst>
@@ -124,9 +138,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1104,7 +1118,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
@@ -1145,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="148.5" spans="1:9">
+    <row r="2" s="1" customFormat="1" ht="216" spans="1:9">
       <c r="A2" s="3">
         <v>1.1</v>
       </c>
@@ -1215,6 +1229,7 @@
       <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="2">
         <v>0</v>
       </c>
@@ -1222,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" ht="256.5" spans="1:9">
+    <row r="5" s="2" customFormat="1" ht="229.5" spans="1:9">
       <c r="A5" s="5">
         <v>1.2</v>
       </c>
@@ -1241,7 +1256,7 @@
       <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="2">
@@ -1259,7 +1274,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="http://181.181.0.33:22020/api/acs/v1/door_ban/insert" tooltip="http://181.181.0.33:22020/api/acs/v1/door_ban/insert"/>
-    <hyperlink ref="D4" r:id="rId2" display="http://181.181.0.33:22020/api/acs/v1/door_ban/" tooltip="http://181.181.0.33:22020/api/acs/v1/door_ban/"/>
+    <hyperlink ref="D4" r:id="rId2" display="http://181.181.0.33:22020/api/acs/v1/door_ban/?id=66" tooltip="http://181.181.0.33:22020/api/acs/v1/door_ban/?id=66"/>
     <hyperlink ref="D3" r:id="rId3" display="http://181.181.0.33:22020/api/acs/v1/door_ban/state" tooltip="http://181.181.0.33:22020/api/acs/v1/door_ban/state"/>
     <hyperlink ref="D5" r:id="rId4" display="http://181.181.0.33:22020/api/acs/v1/door_ban/update" tooltip="http://181.181.0.166:22020/api/acs/v1/door_ban/update"/>
   </hyperlinks>

</xml_diff>